<commit_message>
Added final sprint 2 deliverable files.
</commit_message>
<xml_diff>
--- a/Documents/Test Cases/Sprint 2 Test Cases.xlsx
+++ b/Documents/Test Cases/Sprint 2 Test Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shady\Desktop\grad_school_stuff\class\cs691 capstone\repo\integ_merge\Documents\Test Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32CB897D-CF76-43A1-8493-BEC63A14D66D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0245D650-68D4-4A4D-B379-A5DB2E3CB94A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4335" yWindow="1695" windowWidth="21765" windowHeight="13110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29805" yWindow="2490" windowWidth="21765" windowHeight="13110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 2" sheetId="3" r:id="rId1"/>
@@ -141,7 +141,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,6 +163,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -178,7 +191,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -219,18 +232,7 @@
         <color theme="1"/>
       </left>
       <right/>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -239,9 +241,7 @@
       <right style="thin">
         <color theme="1"/>
       </right>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -249,27 +249,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -278,17 +261,409 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="1"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -299,6 +674,24 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FEC42CDC-23B3-4270-9150-8A37CC2C3A1A}" name="Table1" displayName="Table1" ref="A1:I5" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" tableBorderDxfId="11">
+  <autoFilter ref="A1:I5" xr:uid="{FEC42CDC-23B3-4270-9150-8A37CC2C3A1A}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{CC2AA8E3-4294-4354-AB32-791529BDB355}" name="Test ID" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{102F0131-9C84-4978-B1C4-BEC115F5E2DD}" name="Story ID" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{273D3D1E-3A6A-4F0C-89BB-6C4110F55909}" name="Feature to Test" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{0EE5B81D-787F-4EE0-B928-66CC14F124C3}" name="Test Case" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{DAD02328-4BA8-428B-8BF7-D6B9C8A67B24}" name="Test Steps" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{28090CEE-552B-4DFC-8902-3B13B90C0834}" name="Expected Result" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{98241BFE-8151-4443-8EA4-872360682750}" name="Actual Result" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{F675B736-CD9C-432B-8755-C747F94E02C7}" name="Pass/Fail" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{51F7AC14-2604-4E81-A388-2D957DD5319B}" name="Comments" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -600,148 +993,148 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5718171-E3A5-43EA-8916-56692BCD3805}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
     <col min="4" max="4" width="38.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="38.7109375" customWidth="1"/>
     <col min="6" max="6" width="37.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="38.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" customWidth="1"/>
     <col min="9" max="9" width="35.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+    <row r="2" spans="1:9" ht="39" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="11"/>
+      <c r="I2" s="7"/>
     </row>
-    <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="39" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="12"/>
+      <c r="I3" s="11"/>
     </row>
-    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+    <row r="4" spans="1:9" ht="39" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="11"/>
+      <c r="I4" s="7"/>
     </row>
-    <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+    <row r="5" spans="1:9" ht="39" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="10" t="s">
         <v>28</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="12" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="11" t="s">
@@ -750,7 +1143,7 @@
       <c r="G5" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="10" t="s">
         <v>8</v>
       </c>
       <c r="I5" s="11" t="s">
@@ -758,32 +1151,36 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="8"/>
+      <c r="B6" s="2"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="11"/>
+      <c r="I6" s="4"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="8"/>
+      <c r="B7" s="2"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="11"/>
+      <c r="I7" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>